<commit_message>
all formula cells mapped
</commit_message>
<xml_diff>
--- a/notebooks/_base/jahreslauf_roebel.xlsx
+++ b/notebooks/_base/jahreslauf_roebel.xlsx
@@ -4,7 +4,7 @@
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="e" sheetId="1" state="visible" r:id="rId2"/>
@@ -3295,7 +3295,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="danielwittig" id="{24E3A41C-FF51-BD1A-4492-24F74325823C}" userId="danielwittig" providerId="Teamlab"/>
+  <person displayName="danielwittig" id="{AB5AC3E2-54A4-DBB5-A774-D835F5B49BEB}" userId="danielwittig" providerId="Teamlab"/>
 </personList>
 </file>
 
@@ -3755,15 +3755,15 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="K6" dT="2024-01-20T20:55:16.61Z" personId="{24E3A41C-FF51-BD1A-4492-24F74325823C}" id="{51865848-22AF-0CF2-00B8-EC01B3B44148}" done="0">
+  <threadedComment ref="K6" dT="2024-01-20T20:55:16.61Z" personId="{AB5AC3E2-54A4-DBB5-A774-D835F5B49BEB}" id="{51865848-22AF-0CF2-00B8-EC01B3B44148}" done="0">
     <text xml:space="preserve">eingefügt aus technischen Gründen, um die Bedeutung von Spalte F auszulesen. DW
 </text>
   </threadedComment>
-  <threadedComment ref="C98" dT="2024-01-19T09:30:47.45Z" personId="{24E3A41C-FF51-BD1A-4492-24F74325823C}" id="{AE29D719-1BC3-5689-F671-0C7F00F4C071}" done="0">
+  <threadedComment ref="C98" dT="2024-01-19T09:30:47.45Z" personId="{AB5AC3E2-54A4-DBB5-A774-D835F5B49BEB}" id="{AE29D719-1BC3-5689-F671-0C7F00F4C071}" done="0">
     <text xml:space="preserve">edit dw
 </text>
   </threadedComment>
-  <threadedComment ref="C99" dT="2024-01-19T09:30:28.71Z" personId="{24E3A41C-FF51-BD1A-4492-24F74325823C}" id="{E9A40895-7ABA-4DD2-7DDF-BC2D530EBD2A}" done="0">
+  <threadedComment ref="C99" dT="2024-01-19T09:30:28.71Z" personId="{AB5AC3E2-54A4-DBB5-A774-D835F5B49BEB}" id="{E9A40895-7ABA-4DD2-7DDF-BC2D530EBD2A}" done="0">
     <text xml:space="preserve">edit dw
 </text>
   </threadedComment>
@@ -3777,7 +3777,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="P1" zoomScale="150" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="R1" zoomScale="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Y6" activeCellId="0" sqref="Y6"/>
     </sheetView>
@@ -4059,6 +4059,7 @@
       <c r="W3" s="42"/>
       <c r="X3" s="42"/>
       <c r="Y3" s="42"/>
+      <c r="Z3" s="9"/>
       <c r="AA3" s="17"/>
       <c r="AB3" s="17"/>
       <c r="AC3" s="17"/>
@@ -4189,6 +4190,7 @@
         <v>33</v>
       </c>
       <c r="Y4" s="51"/>
+      <c r="Z4" s="9"/>
       <c r="AA4" s="53"/>
       <c r="AB4" s="53"/>
       <c r="AC4" s="53"/>
@@ -4321,9 +4323,7 @@
       <c r="Y5" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="Z5" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z5" s="9"/>
       <c r="AA5" s="53"/>
       <c r="AB5" s="53"/>
       <c r="AC5" s="53"/>
@@ -4451,7 +4451,7 @@
         <v>39</v>
       </c>
       <c r="X6" s="51"/>
-      <c r="Z6" s="53"/>
+      <c r="Z6" s="9"/>
       <c r="AA6" s="53"/>
       <c r="AB6" s="53"/>
       <c r="AC6" s="53"/>
@@ -4582,7 +4582,7 @@
       <c r="X7" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="Z7" s="53"/>
+      <c r="Z7" s="9"/>
       <c r="AA7" s="53"/>
       <c r="AB7" s="53"/>
       <c r="AC7" s="53"/>
@@ -4713,6 +4713,7 @@
       <c r="Y8" s="51" t="s">
         <v>45</v>
       </c>
+      <c r="Z8" s="9"/>
       <c r="AA8" s="53"/>
       <c r="AB8" s="53"/>
       <c r="AC8" s="53"/>
@@ -4844,6 +4845,7 @@
       <c r="Y9" s="51" t="s">
         <v>1</v>
       </c>
+      <c r="Z9" s="9"/>
       <c r="AA9" s="53"/>
       <c r="AB9" s="53"/>
       <c r="AC9" s="53"/>
@@ -4974,6 +4976,7 @@
         <v>50</v>
       </c>
       <c r="Y10" s="51"/>
+      <c r="Z10" s="9"/>
       <c r="AA10" s="53"/>
       <c r="AB10" s="53"/>
       <c r="AC10" s="53"/>
@@ -5103,6 +5106,7 @@
         <v>53</v>
       </c>
       <c r="Y11" s="51"/>
+      <c r="Z11" s="9"/>
       <c r="AA11" s="53"/>
       <c r="AB11" s="53"/>
       <c r="AC11" s="53"/>
@@ -5232,6 +5236,7 @@
         <v>57</v>
       </c>
       <c r="Y12" s="68"/>
+      <c r="Z12" s="9"/>
       <c r="AA12" s="53"/>
       <c r="AB12" s="53"/>
       <c r="AC12" s="53"/>
@@ -5362,6 +5367,7 @@
         <v>57</v>
       </c>
       <c r="Y13" s="68"/>
+      <c r="Z13" s="9"/>
       <c r="AA13" s="53"/>
       <c r="AB13" s="53"/>
       <c r="AC13" s="53"/>
@@ -5491,6 +5497,7 @@
         <v>60</v>
       </c>
       <c r="Y14" s="51"/>
+      <c r="Z14" s="9"/>
       <c r="AA14" s="53"/>
       <c r="AB14" s="53"/>
       <c r="AC14" s="53"/>
@@ -5620,7 +5627,7 @@
         <v>63</v>
       </c>
       <c r="Y15" s="51"/>
-      <c r="Z15" s="53"/>
+      <c r="Z15" s="9"/>
       <c r="AA15" s="53"/>
       <c r="AB15" s="53"/>
       <c r="AC15" s="53"/>
@@ -5751,6 +5758,7 @@
         <v>65</v>
       </c>
       <c r="Y16" s="53"/>
+      <c r="Z16" s="9"/>
       <c r="AA16" s="53"/>
       <c r="AB16" s="53"/>
       <c r="AC16" s="53"/>
@@ -5880,6 +5888,7 @@
         <v>65</v>
       </c>
       <c r="Y17" s="51"/>
+      <c r="Z17" s="9"/>
       <c r="AA17" s="53"/>
       <c r="AB17" s="53"/>
       <c r="AC17" s="53"/>
@@ -6010,6 +6019,7 @@
         <v>68</v>
       </c>
       <c r="Y18" s="51"/>
+      <c r="Z18" s="9"/>
       <c r="AA18" s="53"/>
       <c r="AB18" s="53"/>
       <c r="AC18" s="53"/>
@@ -6136,6 +6146,7 @@
         <v>70</v>
       </c>
       <c r="Y19" s="51"/>
+      <c r="Z19" s="9"/>
       <c r="AA19" s="53"/>
       <c r="AB19" s="53"/>
       <c r="AC19" s="53"/>
@@ -6265,6 +6276,7 @@
         <v>73</v>
       </c>
       <c r="Y20" s="51"/>
+      <c r="Z20" s="9"/>
       <c r="AA20" s="53"/>
       <c r="AB20" s="53"/>
       <c r="AC20" s="53"/>
@@ -6395,6 +6407,7 @@
         <v>65</v>
       </c>
       <c r="Y21" s="51"/>
+      <c r="Z21" s="9"/>
       <c r="AA21" s="53"/>
       <c r="AB21" s="51" t="s">
         <v>1</v>
@@ -6526,6 +6539,7 @@
         <v>78</v>
       </c>
       <c r="Y22" s="51"/>
+      <c r="Z22" s="9"/>
       <c r="AA22" s="53"/>
       <c r="AB22" s="53"/>
       <c r="AC22" s="53"/>
@@ -6653,6 +6667,7 @@
         <v>80</v>
       </c>
       <c r="Y23" s="51"/>
+      <c r="Z23" s="9"/>
       <c r="AA23" s="53"/>
       <c r="AB23" s="53"/>
       <c r="AC23" s="53"/>
@@ -6782,6 +6797,7 @@
         <f>t!F114</f>
         <v>0.225618124786824</v>
       </c>
+      <c r="Z24" s="9"/>
       <c r="AA24" s="53"/>
       <c r="AB24" s="53"/>
       <c r="AC24" s="53"/>
@@ -6910,6 +6926,7 @@
       <c r="Y25" s="51" t="s">
         <v>86</v>
       </c>
+      <c r="Z25" s="9"/>
       <c r="AA25" s="53"/>
       <c r="AB25" s="53"/>
       <c r="AC25" s="53"/>
@@ -7030,6 +7047,7 @@
       <c r="W26" s="79"/>
       <c r="X26" s="80"/>
       <c r="Y26" s="80"/>
+      <c r="Z26" s="9"/>
       <c r="AA26" s="16"/>
       <c r="AB26" s="16"/>
       <c r="AC26" s="53"/>
@@ -7153,6 +7171,7 @@
       <c r="W27" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="Z27" s="9"/>
       <c r="AA27" s="16"/>
       <c r="AB27" s="16"/>
       <c r="AC27" s="16"/>
@@ -7276,6 +7295,7 @@
       <c r="W28" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="Z28" s="9"/>
       <c r="AC28" s="16"/>
       <c r="AD28" s="16"/>
       <c r="AE28" s="16"/>
@@ -7397,6 +7417,7 @@
       <c r="W29" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="Z29" s="9"/>
     </row>
     <row r="30" ht="12.800000000000001">
       <c r="A30" s="1">
@@ -7482,6 +7503,7 @@
       <c r="W30" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="Z30" s="9"/>
     </row>
     <row r="31" ht="12.800000000000001">
       <c r="A31" s="1">
@@ -7567,6 +7589,7 @@
       <c r="W31" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Z31" s="9"/>
     </row>
     <row r="32" ht="12.800000000000001">
       <c r="A32" s="1">
@@ -7652,6 +7675,7 @@
       <c r="W32" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="Z32" s="9"/>
     </row>
     <row r="33" ht="12.800000000000001">
       <c r="A33" s="1">
@@ -7737,6 +7761,7 @@
       <c r="W33" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="Z33" s="9"/>
     </row>
     <row r="34" ht="12.800000000000001">
       <c r="A34" s="1">
@@ -58597,7 +58622,7 @@
       <c r="G4" s="109"/>
       <c r="H4" s="110"/>
     </row>
-    <row r="5" s="53" customFormat="1" ht="22.850000000000001">
+    <row r="5" s="53" customFormat="1" ht="24">
       <c r="A5" s="112" t="s">
         <v>113</v>
       </c>
@@ -61625,7 +61650,7 @@
     <row r="118" ht="12.800000000000001">
       <c r="A118" s="137"/>
       <c r="B118" s="148" t="str">
-        <f>B117</f>
+        <f t="shared" ref="B118:B181" si="208">B117</f>
         <v>Verteilung</v>
       </c>
       <c r="C118" s="138" t="s">
@@ -61650,7 +61675,7 @@
     <row r="119" ht="12.800000000000001">
       <c r="A119" s="137"/>
       <c r="B119" s="148" t="str">
-        <f>B118</f>
+        <f t="shared" si="208"/>
         <v>Verteilung</v>
       </c>
       <c r="C119" s="138" t="s">
@@ -61675,7 +61700,7 @@
     <row r="120" ht="12.800000000000001">
       <c r="A120" s="137"/>
       <c r="B120" s="148" t="str">
-        <f>B119</f>
+        <f t="shared" si="208"/>
         <v>Verteilung</v>
       </c>
       <c r="C120" s="138" t="s">
@@ -61700,7 +61725,7 @@
     <row r="121" ht="12.800000000000001">
       <c r="A121" s="137"/>
       <c r="B121" s="148" t="str">
-        <f>B120</f>
+        <f t="shared" si="208"/>
         <v>Verteilung</v>
       </c>
       <c r="C121" s="138" t="s">
@@ -61725,7 +61750,7 @@
     <row r="122" ht="12.800000000000001">
       <c r="A122" s="137"/>
       <c r="B122" s="148" t="str">
-        <f>B121</f>
+        <f t="shared" si="208"/>
         <v>Verteilung</v>
       </c>
       <c r="C122" s="138" t="s">
@@ -61750,7 +61775,7 @@
     <row r="123" ht="12.800000000000001">
       <c r="A123" s="137"/>
       <c r="B123" s="148" t="str">
-        <f>B122</f>
+        <f t="shared" si="208"/>
         <v>Verteilung</v>
       </c>
       <c r="C123" s="138" t="s">
@@ -61773,7 +61798,7 @@
     <row r="124" ht="12.800000000000001">
       <c r="A124" s="137"/>
       <c r="B124" s="148" t="str">
-        <f>B123</f>
+        <f t="shared" si="208"/>
         <v>Verteilung</v>
       </c>
       <c r="C124" s="138" t="s">
@@ -61798,7 +61823,7 @@
     <row r="125" ht="12.800000000000001">
       <c r="A125" s="137"/>
       <c r="B125" s="148" t="str">
-        <f>B124</f>
+        <f t="shared" si="208"/>
         <v>Verteilung</v>
       </c>
       <c r="C125" s="138" t="s">
@@ -61862,7 +61887,7 @@
     <row r="128" ht="12.800000000000001">
       <c r="A128" s="137"/>
       <c r="B128" s="148" t="str">
-        <f>B127</f>
+        <f t="shared" si="208"/>
         <v>Unterverteilung</v>
       </c>
       <c r="C128" s="138" t="s">
@@ -61887,7 +61912,7 @@
     <row r="129" ht="12.800000000000001">
       <c r="A129" s="137"/>
       <c r="B129" s="148" t="str">
-        <f>B128</f>
+        <f t="shared" si="208"/>
         <v>Unterverteilung</v>
       </c>
       <c r="C129" s="138" t="s">
@@ -61912,7 +61937,7 @@
     <row r="130" ht="12.800000000000001">
       <c r="A130" s="137"/>
       <c r="B130" s="148" t="str">
-        <f>B129</f>
+        <f t="shared" si="208"/>
         <v>Unterverteilung</v>
       </c>
       <c r="C130" s="138" t="s">
@@ -61937,7 +61962,7 @@
     <row r="131" ht="12.800000000000001">
       <c r="A131" s="137"/>
       <c r="B131" s="148" t="str">
-        <f>B130</f>
+        <f t="shared" si="208"/>
         <v>Unterverteilung</v>
       </c>
       <c r="C131" s="138" t="s">
@@ -62001,7 +62026,7 @@
     <row r="134" ht="12.800000000000001">
       <c r="A134" s="137"/>
       <c r="B134" s="148" t="str">
-        <f>B133</f>
+        <f t="shared" si="208"/>
         <v>Hauptverteilung</v>
       </c>
       <c r="C134" s="138" t="s">
@@ -62026,7 +62051,7 @@
     <row r="135" ht="12.800000000000001">
       <c r="A135" s="137"/>
       <c r="B135" s="148" t="str">
-        <f>B134</f>
+        <f t="shared" si="208"/>
         <v>Hauptverteilung</v>
       </c>
       <c r="C135" s="138" t="s">
@@ -62051,7 +62076,7 @@
     <row r="136" ht="12.800000000000001">
       <c r="A136" s="137"/>
       <c r="B136" s="148" t="str">
-        <f>B135</f>
+        <f t="shared" si="208"/>
         <v>Hauptverteilung</v>
       </c>
       <c r="C136" s="138" t="s">
@@ -62076,7 +62101,7 @@
     <row r="137" ht="12.800000000000001">
       <c r="A137" s="137"/>
       <c r="B137" s="148" t="str">
-        <f>B136</f>
+        <f t="shared" si="208"/>
         <v>Hauptverteilung</v>
       </c>
       <c r="C137" s="138" t="s">
@@ -62122,7 +62147,7 @@
         <v>326</v>
       </c>
       <c r="D139" s="122">
-        <f t="shared" ref="D139:D140" si="208">D129+D135</f>
+        <f t="shared" ref="D139:D140" si="209">D129+D135</f>
         <v>170.73305728166</v>
       </c>
       <c r="E139" s="1" t="s">
@@ -62140,14 +62165,14 @@
     <row r="140" ht="12.800000000000001">
       <c r="A140" s="137"/>
       <c r="B140" s="148" t="str">
-        <f>B139</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C140" s="138" t="s">
         <v>327</v>
       </c>
       <c r="D140" s="122">
-        <f t="shared" si="208"/>
+        <f t="shared" si="209"/>
         <v>967.54226980174406</v>
       </c>
       <c r="E140" s="1" t="s">
@@ -62165,7 +62190,7 @@
     <row r="141" ht="12.800000000000001">
       <c r="A141" s="137"/>
       <c r="B141" s="148" t="str">
-        <f>B140</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C141" s="138" t="s">
@@ -62190,7 +62215,7 @@
     <row r="142" ht="12.800000000000001">
       <c r="A142" s="137"/>
       <c r="B142" s="148" t="str">
-        <f>B141</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C142" s="138" t="s">
@@ -62215,7 +62240,7 @@
     <row r="143" ht="12.800000000000001">
       <c r="A143" s="137"/>
       <c r="B143" s="148" t="str">
-        <f>B142</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C143" s="138" t="s">
@@ -62240,7 +62265,7 @@
     <row r="144" ht="12.800000000000001">
       <c r="A144" s="137"/>
       <c r="B144" s="148" t="str">
-        <f>B143</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C144" s="138" t="s">
@@ -62265,7 +62290,7 @@
     <row r="145" ht="12.800000000000001">
       <c r="A145" s="137"/>
       <c r="B145" s="148" t="str">
-        <f>B144</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C145" s="138" t="s">
@@ -62290,7 +62315,7 @@
     <row r="146" ht="12.800000000000001">
       <c r="A146" s="137"/>
       <c r="B146" s="148" t="str">
-        <f>B145</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C146" s="138" t="s">
@@ -62315,7 +62340,7 @@
     <row r="147" ht="12.800000000000001">
       <c r="A147" s="137"/>
       <c r="B147" s="148" t="str">
-        <f>B146</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C147" s="138" t="s">
@@ -62342,7 +62367,7 @@
     <row r="148" ht="12.800000000000001">
       <c r="A148" s="137"/>
       <c r="B148" s="148" t="str">
-        <f>B147</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C148" s="138"/>
@@ -62360,7 +62385,7 @@
     <row r="149" ht="12.800000000000001">
       <c r="A149" s="137"/>
       <c r="B149" s="148" t="str">
-        <f>B148</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C149" s="138" t="s">
@@ -62385,7 +62410,7 @@
     <row r="150" ht="12.800000000000001">
       <c r="A150" s="137"/>
       <c r="B150" s="148" t="str">
-        <f>B149</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C150" s="138" t="s">
@@ -62410,7 +62435,7 @@
     <row r="151" ht="12.800000000000001">
       <c r="A151" s="137"/>
       <c r="B151" s="148" t="str">
-        <f>B150</f>
+        <f t="shared" si="208"/>
         <v xml:space="preserve">Verteilung gesamt</v>
       </c>
       <c r="C151" s="138" t="s">
@@ -62548,7 +62573,7 @@
         <v>341</v>
       </c>
       <c r="D157" s="139">
-        <f t="shared" ref="D157:D159" si="209">D153/D$98*100</f>
+        <f t="shared" ref="D157:D159" si="210">D153/D$98*100</f>
         <v>12.2987279458917</v>
       </c>
       <c r="E157" s="1" t="s">
@@ -62572,7 +62597,7 @@
         <v>343</v>
       </c>
       <c r="D158" s="139">
-        <f t="shared" si="209"/>
+        <f t="shared" si="210"/>
         <v>8.5779219863429592</v>
       </c>
       <c r="E158" s="1" t="s">
@@ -62598,7 +62623,7 @@
         <v>344</v>
       </c>
       <c r="D159" s="157">
-        <f t="shared" si="209"/>
+        <f t="shared" si="210"/>
         <v>20.876649932234599</v>
       </c>
       <c r="E159" s="154" t="s">
@@ -62774,7 +62799,7 @@
     <row r="167" ht="12.800000000000001">
       <c r="A167" s="14"/>
       <c r="B167" s="159" t="str">
-        <f>B166</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C167" s="51" t="s">
@@ -62801,7 +62826,7 @@
     <row r="168" ht="12.800000000000001">
       <c r="A168" s="14"/>
       <c r="B168" s="159" t="str">
-        <f>B167</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C168" s="51" t="s">
@@ -62829,7 +62854,7 @@
     <row r="169" ht="12.800000000000001">
       <c r="A169" s="14"/>
       <c r="B169" s="159" t="str">
-        <f>B168</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C169" s="51" t="s">
@@ -62857,7 +62882,7 @@
     <row r="170" ht="12.800000000000001">
       <c r="A170" s="14"/>
       <c r="B170" s="159" t="str">
-        <f>B169</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C170" s="51" t="s">
@@ -62888,7 +62913,7 @@
     <row r="171" ht="12.800000000000001">
       <c r="A171" s="16"/>
       <c r="B171" s="159" t="str">
-        <f>B170</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C171" s="19" t="s">
@@ -62918,7 +62943,7 @@
         <v>1</v>
       </c>
       <c r="B172" s="159" t="str">
-        <f>B171</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C172" s="51" t="s">
@@ -62947,7 +62972,7 @@
     <row r="173" ht="12.800000000000001">
       <c r="A173" s="14"/>
       <c r="B173" s="159" t="str">
-        <f>B172</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C173" s="51" t="s">
@@ -62976,7 +63001,7 @@
     <row r="174" ht="12.800000000000001">
       <c r="A174" s="14"/>
       <c r="B174" s="159" t="str">
-        <f>B173</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C174" s="51" t="s">
@@ -63005,7 +63030,7 @@
     <row r="175" ht="12.800000000000001">
       <c r="A175" s="14"/>
       <c r="B175" s="159" t="str">
-        <f>B174</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C175" s="51" t="s">
@@ -63033,7 +63058,7 @@
     <row r="176" ht="12.800000000000001">
       <c r="A176" s="14"/>
       <c r="B176" s="159" t="str">
-        <f>B175</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C176" s="51" t="s">
@@ -63061,7 +63086,7 @@
     <row r="177" ht="12.800000000000001">
       <c r="A177" s="14"/>
       <c r="B177" s="159" t="str">
-        <f>B176</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C177" s="51" t="s">
@@ -63089,7 +63114,7 @@
     <row r="178" ht="12.800000000000001">
       <c r="A178" s="14"/>
       <c r="B178" s="159" t="str">
-        <f>B177</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C178" s="51" t="s">
@@ -63118,7 +63143,7 @@
     <row r="179" ht="12.800000000000001">
       <c r="A179" s="14"/>
       <c r="B179" s="159" t="str">
-        <f>B178</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C179" s="51" t="s">
@@ -63149,7 +63174,7 @@
         <v>1</v>
       </c>
       <c r="B180" s="159" t="str">
-        <f>B179</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C180" s="51" t="s">
@@ -63180,7 +63205,7 @@
         <v>1</v>
       </c>
       <c r="B181" s="159" t="str">
-        <f>B180</f>
+        <f t="shared" si="208"/>
         <v>Investition</v>
       </c>
       <c r="C181" s="19" t="s">
@@ -63251,7 +63276,7 @@
     <row r="184" ht="12.800000000000001">
       <c r="A184" s="16"/>
       <c r="B184" s="159" t="str">
-        <f>B183</f>
+        <f t="shared" ref="B182:B187" si="211">B183</f>
         <v xml:space="preserve">laufende Kosten</v>
       </c>
       <c r="C184" s="51" t="s">
@@ -63279,7 +63304,7 @@
     <row r="185" ht="12.800000000000001">
       <c r="A185" s="16"/>
       <c r="B185" s="159" t="str">
-        <f>B184</f>
+        <f t="shared" si="211"/>
         <v xml:space="preserve">laufende Kosten</v>
       </c>
       <c r="C185" s="51" t="s">
@@ -63309,7 +63334,7 @@
     <row r="186" ht="12.800000000000001">
       <c r="A186" s="16"/>
       <c r="B186" s="159" t="str">
-        <f>B185</f>
+        <f t="shared" si="211"/>
         <v xml:space="preserve">laufende Kosten</v>
       </c>
       <c r="C186" s="51" t="s">
@@ -63341,7 +63366,7 @@
         <v>1</v>
       </c>
       <c r="B187" s="159" t="str">
-        <f>B186</f>
+        <f t="shared" si="211"/>
         <v xml:space="preserve">laufende Kosten</v>
       </c>
       <c r="C187" s="51" t="s">
@@ -63393,7 +63418,7 @@
         <v>362</v>
       </c>
       <c r="D189" s="127">
-        <f t="shared" ref="D189:D198" si="210">D171/F171/E$3</f>
+        <f t="shared" ref="D189:D198" si="212">D171/F171/E$3</f>
         <v>15.936059570271301</v>
       </c>
       <c r="E189" s="1" t="s">
@@ -63403,7 +63428,7 @@
         <v>382</v>
       </c>
       <c r="G189" s="163">
-        <f t="shared" ref="G189:G198" si="211">D189/D$210</f>
+        <f t="shared" ref="G189:G198" si="213">D189/D$210</f>
         <v>0.021896759821409598</v>
       </c>
       <c r="H189" s="51" t="s">
@@ -63425,7 +63450,7 @@
         <v>363</v>
       </c>
       <c r="D190" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>0.39742689485207999</v>
       </c>
       <c r="E190" s="1" t="s">
@@ -63435,7 +63460,7 @@
         <v>382</v>
       </c>
       <c r="G190" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.00054607986527477901</v>
       </c>
       <c r="H190" s="51" t="s">
@@ -63457,7 +63482,7 @@
         <v>364</v>
       </c>
       <c r="D191" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>0.99249815354627402</v>
       </c>
       <c r="E191" s="1" t="s">
@@ -63467,7 +63492,7 @@
         <v>382</v>
       </c>
       <c r="G191" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.0013637307011538299</v>
       </c>
       <c r="H191" s="51" t="s">
@@ -63489,7 +63514,7 @@
         <v>151</v>
       </c>
       <c r="D192" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>156.33306302598399</v>
       </c>
       <c r="E192" s="1" t="s">
@@ -63499,7 +63524,7 @@
         <v>382</v>
       </c>
       <c r="G192" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.21480765167389301</v>
       </c>
       <c r="H192" s="51" t="s">
@@ -63521,7 +63546,7 @@
         <v>365</v>
       </c>
       <c r="D193" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>94.297407112695495</v>
       </c>
       <c r="E193" s="1" t="s">
@@ -63531,7 +63556,7 @@
         <v>382</v>
       </c>
       <c r="G193" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.12956827038851401</v>
       </c>
       <c r="H193" s="51" t="s">
@@ -63553,7 +63578,7 @@
         <v>366</v>
       </c>
       <c r="D194" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>0</v>
       </c>
       <c r="E194" s="1" t="s">
@@ -63563,7 +63588,7 @@
         <v>382</v>
       </c>
       <c r="G194" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0</v>
       </c>
       <c r="H194" s="51" t="s">
@@ -63585,7 +63610,7 @@
         <v>367</v>
       </c>
       <c r="D195" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>0.34483759249988399</v>
       </c>
       <c r="E195" s="1" t="s">
@@ -63595,7 +63620,7 @@
         <v>382</v>
       </c>
       <c r="G195" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.00047382013772395302</v>
       </c>
       <c r="H195" s="51" t="s">
@@ -63617,7 +63642,7 @@
         <v>368</v>
       </c>
       <c r="D196" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>146.18324694565999</v>
       </c>
       <c r="E196" s="1" t="s">
@@ -63627,7 +63652,7 @@
         <v>382</v>
       </c>
       <c r="G196" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.20086141333547</v>
       </c>
       <c r="H196" s="51" t="s">
@@ -63649,7 +63674,7 @@
         <v>369</v>
       </c>
       <c r="D197" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>73.610002660282007</v>
       </c>
       <c r="E197" s="1" t="s">
@@ -63659,7 +63684,7 @@
         <v>382</v>
       </c>
       <c r="G197" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.101142979642996</v>
       </c>
       <c r="H197" s="51" t="s">
@@ -63683,7 +63708,7 @@
         <v>370</v>
       </c>
       <c r="D198" s="127">
-        <f t="shared" si="210"/>
+        <f t="shared" si="212"/>
         <v>23.9423662255126</v>
       </c>
       <c r="E198" s="1" t="s">
@@ -63693,7 +63718,7 @@
         <v>382</v>
       </c>
       <c r="G198" s="163">
-        <f t="shared" si="211"/>
+        <f t="shared" si="213"/>
         <v>0.032897733626340402</v>
       </c>
       <c r="H198" s="51" t="s">
@@ -63787,7 +63812,7 @@
         <v>373</v>
       </c>
       <c r="D202" s="122">
-        <f t="shared" ref="D202:D206" si="212">D183/E$3</f>
+        <f t="shared" ref="D202:D206" si="214">D183/E$3</f>
         <v>28.058540427326001</v>
       </c>
       <c r="E202" s="1" t="s">
@@ -63809,7 +63834,7 @@
         <v>375</v>
       </c>
       <c r="D203" s="122">
-        <f t="shared" si="212"/>
+        <f t="shared" si="214"/>
         <v>340.009934563493</v>
       </c>
       <c r="E203" s="1" t="s">
@@ -63831,7 +63856,7 @@
         <v>376</v>
       </c>
       <c r="D204" s="122">
-        <f t="shared" si="212"/>
+        <f t="shared" si="214"/>
         <v>-132.603874479762</v>
       </c>
       <c r="E204" s="1" t="s">
@@ -63853,7 +63878,7 @@
         <v>386</v>
       </c>
       <c r="D205" s="122">
-        <f t="shared" si="212"/>
+        <f t="shared" si="214"/>
         <v>2.4010471781305101</v>
       </c>
       <c r="E205" s="1" t="s">
@@ -63877,7 +63902,7 @@
         <v>379</v>
       </c>
       <c r="D206" s="122">
-        <f t="shared" si="212"/>
+        <f t="shared" si="214"/>
         <v>81.2182741116751</v>
       </c>
       <c r="E206" s="1" t="s">
@@ -64659,27 +64684,27 @@
         <v>6587.7474857192501</v>
       </c>
       <c r="G21" s="186">
-        <f t="shared" ref="G21:G31" si="213">$F21*2</f>
+        <f t="shared" ref="G21:G31" si="215">$F21*2</f>
         <v>13175.4949714385</v>
       </c>
       <c r="H21" s="188">
-        <f t="shared" ref="H21:H31" si="214">(G21/4200/(2*D$17)/(60-30)*4/PI())^0.5</f>
+        <f t="shared" ref="H21:H31" si="216">(G21/4200/(2*D$17)/(60-30)*4/PI())^0.5</f>
         <v>0.235530761220554</v>
       </c>
       <c r="I21" s="186">
-        <f t="shared" ref="I21:I31" si="215">(0.657/H21-0.058)*D$17^1.92/10000*E21*1.5</f>
+        <f t="shared" ref="I21:I31" si="217">(0.657/H21-0.058)*D$17^1.92/10000*E21*1.5</f>
         <v>1.7966774646497301</v>
       </c>
       <c r="J21" s="186">
-        <f t="shared" ref="J21:J31" si="216">(0.657/H21-0.058)*(2*D$17)^1.92/10000*E21*1.5</f>
+        <f t="shared" ref="J21:J31" si="218">(0.657/H21-0.058)*(2*D$17)^1.92/10000*E21*1.5</f>
         <v>6.79904181652575</v>
       </c>
       <c r="K21" s="189">
-        <f t="shared" ref="K21:K31" si="217">I21*10^5*PI()/4*$H21^2*D$17/1000*2/0.75</f>
+        <f t="shared" ref="K21:K31" si="219">I21*10^5*PI()/4*$H21^2*D$17/1000*2/0.75</f>
         <v>25.0498570378724</v>
       </c>
       <c r="L21" s="190">
-        <f t="shared" ref="L21:L31" si="218">J21*10^5*PI()/4*$H21^2*(2*D$17)/1000*2/0.75</f>
+        <f t="shared" ref="L21:L31" si="220">J21*10^5*PI()/4*$H21^2*(2*D$17)/1000*2/0.75</f>
         <v>189.588870400497</v>
       </c>
       <c r="M21" s="190" t="s">
@@ -64690,23 +64715,23 @@
         <v>0.71527777777777801</v>
       </c>
       <c r="O21" s="45">
-        <f t="shared" ref="O21:O31" si="219">E21/(2*D$17)/3600</f>
+        <f t="shared" ref="O21:O31" si="221">E21/(2*D$17)/3600</f>
         <v>0.35763888888888901</v>
       </c>
       <c r="P21" s="186">
-        <f t="shared" ref="P21:P31" si="220">(50+20)*2*PI()*$G$16*E21/LN(1+$D$16*2/H21)/1000</f>
+        <f t="shared" ref="P21:P31" si="222">(50+20)*2*PI()*$G$16*E21/LN(1+$D$16*2/H21)/1000</f>
         <v>101.96563843781701</v>
       </c>
       <c r="Q21" s="186">
-        <f t="shared" ref="Q21:Q31" si="221">P21*24*180</f>
+        <f t="shared" ref="Q21:Q31" si="223">P21*24*180</f>
         <v>440491.55805137003</v>
       </c>
       <c r="R21" s="190">
-        <f t="shared" ref="R21:R32" si="222">P21/F21*100</f>
+        <f t="shared" ref="R21:R32" si="224">P21/F21*100</f>
         <v>1.5478073295744199</v>
       </c>
       <c r="S21" s="45">
-        <f t="shared" ref="S21:S31" si="223">1-R21/100</f>
+        <f t="shared" ref="S21:S31" si="225">1-R21/100</f>
         <v>0.98452192670425598</v>
       </c>
       <c r="T21" s="2">
@@ -64731,27 +64756,27 @@
         <v>573.52154581555806</v>
       </c>
       <c r="G22" s="48">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>1147.04309163112</v>
       </c>
       <c r="H22" s="176">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.069495075759567995</v>
       </c>
       <c r="I22" s="48">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>7.48048186412744</v>
       </c>
       <c r="J22" s="48">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>28.307868274999599</v>
       </c>
       <c r="K22" s="192">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>9.0798254437240509</v>
       </c>
       <c r="L22" s="63">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>68.720306335750095</v>
       </c>
       <c r="M22" s="63" t="s">
@@ -64762,23 +64787,23 @@
         <v>0.86574074074074103</v>
       </c>
       <c r="O22" s="193">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.43287037037037002</v>
       </c>
       <c r="P22" s="48">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>52.175560702055897</v>
       </c>
       <c r="Q22" s="48">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>225398.422232882</v>
       </c>
       <c r="R22" s="63">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>9.0974020213767801</v>
       </c>
       <c r="S22" s="193">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.90902597978623201</v>
       </c>
       <c r="T22" s="1">
@@ -64847,27 +64872,27 @@
         <v>2004.7419799679001</v>
       </c>
       <c r="G23" s="48">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>4009.4839599357902</v>
       </c>
       <c r="H23" s="176">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.12992969114910499</v>
       </c>
       <c r="I23" s="48">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>2.27708768113279</v>
       </c>
       <c r="J23" s="48">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>8.61702485200132</v>
       </c>
       <c r="K23" s="192">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>9.6613190824013806</v>
       </c>
       <c r="L23" s="63">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>73.121318362893902</v>
       </c>
       <c r="M23" s="63" t="s">
@@ -64878,23 +64903,23 @@
         <v>0.49537037037037002</v>
       </c>
       <c r="O23" s="193">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.24768518518518501</v>
       </c>
       <c r="P23" s="48">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>45.0549505489819</v>
       </c>
       <c r="Q23" s="48">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>194637.38637160201</v>
       </c>
       <c r="R23" s="63">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>2.2474189197007499</v>
       </c>
       <c r="S23" s="193">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.97752581080299195</v>
       </c>
       <c r="T23" s="1">
@@ -64961,27 +64986,27 @@
         <v>500.78804416327301</v>
       </c>
       <c r="G24" s="186">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>1001.57608832655</v>
       </c>
       <c r="H24" s="188">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.064939081208845797</v>
       </c>
       <c r="I24" s="186">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>7.6445125628675203</v>
       </c>
       <c r="J24" s="186">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>28.928598262362801</v>
       </c>
       <c r="K24" s="189">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>8.1021809416719499</v>
       </c>
       <c r="L24" s="190">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>61.321041880185099</v>
       </c>
       <c r="M24" s="190" t="s">
@@ -64992,23 +65017,23 @@
         <v>0.82638888888888895</v>
       </c>
       <c r="O24" s="45">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.41319444444444398</v>
       </c>
       <c r="P24" s="186">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>47.818361007727503</v>
       </c>
       <c r="Q24" s="186">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>206575.31955338299</v>
       </c>
       <c r="R24" s="190">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>9.5486227287281498</v>
       </c>
       <c r="S24" s="45">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.90451377271271804</v>
       </c>
       <c r="T24" s="2">
@@ -65022,7 +65047,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="48">
-        <f t="shared" ref="D25:D26" si="224">D8</f>
+        <f t="shared" ref="D25:D26" si="226">D8</f>
         <v>300.67450000000002</v>
       </c>
       <c r="E25" s="191">
@@ -65033,27 +65058,27 @@
         <v>377.97573809466098</v>
       </c>
       <c r="G25" s="48">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>755.95147618932197</v>
       </c>
       <c r="H25" s="176">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.056417147702140402</v>
       </c>
       <c r="I25" s="48">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>4.4399449808786997</v>
       </c>
       <c r="J25" s="48">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>16.801775600804898</v>
       </c>
       <c r="K25" s="192">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>3.5517280026398099</v>
       </c>
       <c r="L25" s="63">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>26.881115487894601</v>
       </c>
       <c r="M25" s="63" t="s">
@@ -65064,23 +65089,23 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="O25" s="193">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.20833333333333301</v>
       </c>
       <c r="P25" s="48">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>22.2120784994564</v>
       </c>
       <c r="Q25" s="48">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>95956.179117651802</v>
       </c>
       <c r="R25" s="63">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>5.8765884316875399</v>
       </c>
       <c r="S25" s="193">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.94123411568312398</v>
       </c>
       <c r="T25" s="1">
@@ -65138,7 +65163,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="48">
-        <f t="shared" si="224"/>
+        <f t="shared" si="226"/>
         <v>97.695499999999996</v>
       </c>
       <c r="E26" s="191">
@@ -65149,27 +65174,27 @@
         <v>122.812306068612</v>
       </c>
       <c r="G26" s="48">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>245.62461213722401</v>
       </c>
       <c r="H26" s="176">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.032158820149438598</v>
       </c>
       <c r="I26" s="48">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>5.8977819850519602</v>
       </c>
       <c r="J26" s="48">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>22.318566982715499</v>
       </c>
       <c r="K26" s="192">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>1.53295281751143</v>
       </c>
       <c r="L26" s="63">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>11.6020938806099</v>
       </c>
       <c r="M26" s="63" t="s">
@@ -65180,23 +65205,23 @@
         <v>0.31481481481481499</v>
       </c>
       <c r="O26" s="193">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.157407407407407</v>
       </c>
       <c r="P26" s="48">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>12.478506744545699</v>
       </c>
       <c r="Q26" s="48">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>53907.1491364373</v>
       </c>
       <c r="R26" s="63">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>10.1606322232678</v>
       </c>
       <c r="S26" s="193">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.89839367776732204</v>
       </c>
       <c r="T26" s="1">
@@ -65265,27 +65290,27 @@
         <v>425.66983753878202</v>
       </c>
       <c r="G27" s="48">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>851.33967507756404</v>
       </c>
       <c r="H27" s="176">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.059870874622070698</v>
       </c>
       <c r="I27" s="48">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>5.9485001133981497</v>
       </c>
       <c r="J27" s="48">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>22.510496075313601</v>
       </c>
       <c r="K27" s="192">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>5.3589356124224699</v>
       </c>
       <c r="L27" s="63">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>40.558896115539099</v>
       </c>
       <c r="M27" s="63" t="s">
@@ -65296,23 +65321,23 @@
         <v>0.592592592592593</v>
       </c>
       <c r="O27" s="193">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.296296296296296</v>
       </c>
       <c r="P27" s="48">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>32.690789735768803</v>
       </c>
       <c r="Q27" s="48">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>141224.211658521</v>
       </c>
       <c r="R27" s="63">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>7.6798464097870998</v>
       </c>
       <c r="S27" s="193">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.92320153590212894</v>
       </c>
       <c r="T27" s="1">
@@ -65381,27 +65406,27 @@
         <v>572.32919332945505</v>
       </c>
       <c r="G28" s="48">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>1144.6583866589101</v>
       </c>
       <c r="H28" s="176">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.069422797970111597</v>
       </c>
       <c r="I28" s="48">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>4.1846483241776999</v>
       </c>
       <c r="J28" s="48">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>15.8356741837831</v>
       </c>
       <c r="K28" s="192">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>5.0687754491938302</v>
       </c>
       <c r="L28" s="63">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>38.362830185958302</v>
       </c>
       <c r="M28" s="63" t="s">
@@ -65412,23 +65437,23 @@
         <v>0.483796296296296</v>
       </c>
       <c r="O28" s="193">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.241898148148148</v>
       </c>
       <c r="P28" s="48">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>29.138564596941301</v>
       </c>
       <c r="Q28" s="48">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>125878.599058786</v>
       </c>
       <c r="R28" s="63">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>5.0912245848287503</v>
       </c>
       <c r="S28" s="193">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.94908775415171298</v>
       </c>
       <c r="T28" s="1">
@@ -65497,27 +65522,27 @@
         <v>213.431095012443</v>
       </c>
       <c r="G29" s="48">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>426.86219002488502</v>
       </c>
       <c r="H29" s="176">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.042394352836438401</v>
       </c>
       <c r="I29" s="48">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>5.1271117110865401</v>
       </c>
       <c r="J29" s="48">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>19.402172959559099</v>
       </c>
       <c r="K29" s="192">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>2.3159472312133702</v>
       </c>
       <c r="L29" s="63">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>17.5281567000191</v>
       </c>
       <c r="M29" s="63" t="s">
@@ -65528,23 +65553,23 @@
         <v>0.36111111111111099</v>
       </c>
       <c r="O29" s="193">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.180555555555556</v>
       </c>
       <c r="P29" s="48">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>16.457688585559001</v>
       </c>
       <c r="Q29" s="48">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>71097.214689614702</v>
       </c>
       <c r="R29" s="63">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>7.7110078944211597</v>
       </c>
       <c r="S29" s="193">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.92288992105578804</v>
       </c>
       <c r="T29" s="1">
@@ -65611,27 +65636,27 @@
         <v>1597.75233137806</v>
       </c>
       <c r="G30" s="186">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>3195.5046627561301</v>
       </c>
       <c r="H30" s="188">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.115993564265783</v>
       </c>
       <c r="I30" s="186">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>5.2508950453726104</v>
       </c>
       <c r="J30" s="186">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>19.8705976393132</v>
       </c>
       <c r="K30" s="189">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>17.755830265747299</v>
       </c>
       <c r="L30" s="190">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>134.38431197497599</v>
       </c>
       <c r="M30" s="190" t="s">
@@ -65642,23 +65667,23 @@
         <v>1.0185185185185199</v>
       </c>
       <c r="O30" s="45">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.50925925925925897</v>
       </c>
       <c r="P30" s="186">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>85.562445805151398</v>
       </c>
       <c r="Q30" s="186">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>369629.76587825402</v>
       </c>
       <c r="R30" s="190">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>5.3551757756694203</v>
       </c>
       <c r="S30" s="45">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.94644824224330604</v>
       </c>
       <c r="T30" s="2">
@@ -65681,27 +65706,27 @@
         <v>764.297943592043</v>
       </c>
       <c r="G31" s="186">
-        <f t="shared" si="213"/>
+        <f t="shared" si="215"/>
         <v>1528.5958871840901</v>
       </c>
       <c r="H31" s="188">
-        <f t="shared" si="214"/>
+        <f t="shared" si="216"/>
         <v>0.080225144733396397</v>
       </c>
       <c r="I31" s="186">
-        <f t="shared" si="215"/>
+        <f t="shared" si="217"/>
         <v>2.3541074470368</v>
       </c>
       <c r="J31" s="186">
-        <f t="shared" si="216"/>
+        <f t="shared" si="218"/>
         <v>8.9084854059313496</v>
       </c>
       <c r="K31" s="189">
-        <f t="shared" si="217"/>
+        <f t="shared" si="219"/>
         <v>3.8079142450051702</v>
       </c>
       <c r="L31" s="190">
-        <f t="shared" si="218"/>
+        <f t="shared" si="220"/>
         <v>28.820051116499702</v>
       </c>
       <c r="M31" s="190" t="s">
@@ -65712,23 +65737,23 @@
         <v>0.31481481481481499</v>
       </c>
       <c r="O31" s="45">
-        <f t="shared" si="219"/>
+        <f t="shared" si="221"/>
         <v>0.157407407407407</v>
       </c>
       <c r="P31" s="186">
-        <f t="shared" si="220"/>
+        <f t="shared" si="222"/>
         <v>20.7321204974062</v>
       </c>
       <c r="Q31" s="186">
-        <f t="shared" si="221"/>
+        <f t="shared" si="223"/>
         <v>89562.760548795006</v>
       </c>
       <c r="R31" s="190">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>2.7125704931207202</v>
       </c>
       <c r="S31" s="45">
-        <f t="shared" si="223"/>
+        <f t="shared" si="225"/>
         <v>0.97287429506879297</v>
       </c>
       <c r="T31" s="2">
@@ -65779,7 +65804,7 @@
         <v>2014358.5662972999</v>
       </c>
       <c r="R32" s="196">
-        <f t="shared" si="222"/>
+        <f t="shared" si="224"/>
         <v>4.9339449933567598</v>
       </c>
       <c r="S32" s="173"/>
@@ -65850,7 +65875,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" aboveAverage="0" operator="greaterThan" rank="0" text="" id="{004C002B-00EC-4F2A-9074-008800D00006}">
+          <x14:cfRule type="cellIs" priority="2" aboveAverage="0" operator="greaterThan" rank="0" text="" id="{00A90033-0057-4542-A2B9-0043006200FF}">
             <xm:f>10</xm:f>
             <x14:dxf>
               <font>
@@ -66922,7 +66947,7 @@
         <v>250.33928571428601</v>
       </c>
       <c r="D16" s="214">
-        <f t="shared" ref="D16:D24" si="225">B$4/B$6/2</f>
+        <f t="shared" ref="D16:D24" si="227">B$4/B$6/2</f>
         <v>3.2261933049592901</v>
       </c>
       <c r="E16" s="215">
@@ -66930,35 +66955,35 @@
         <v>90.542488981569207</v>
       </c>
       <c r="F16" s="216">
-        <f t="shared" ref="F16:F17" si="226">(E16*4/PI()/4.2/(60-30)/1000/B$8)^0.5</f>
+        <f t="shared" ref="F16:F17" si="228">(E16*4/PI()/4.2/(60-30)/1000/B$8)^0.5</f>
         <v>0.0225454936359708</v>
       </c>
       <c r="G16" s="217">
-        <f t="shared" ref="G16:G17" si="227">0.216/(B$8*F16/((1.5556*EXP(-0.0318393*B$9)+0.2374))/10^(-6))^0.2*1/(F16)*B$8^2*(-0.0040125*B$9^2-0.028625*B$9+1000.3875)/2/100000</f>
+        <f t="shared" ref="G16:G17" si="229">0.216/(B$8*F16/((1.5556*EXP(-0.0318393*B$9)+0.2374))/10^(-6))^0.2*1/(F16)*B$8^2*(-0.0040125*B$9^2-0.028625*B$9+1000.3875)/2/100000</f>
         <v>0.0157153884534184</v>
       </c>
       <c r="H16" s="218">
-        <f t="shared" ref="H16:H17" si="228">G16*C$16*2</f>
+        <f t="shared" ref="H16:H17" si="230">G16*C$16*2</f>
         <v>7.86835824030259</v>
       </c>
       <c r="I16" s="219">
-        <f t="shared" ref="I16:I17" si="229">H16*10^5*PI()/4*F16^2*B$8/1000/0.75</f>
+        <f t="shared" ref="I16:I17" si="231">H16*10^5*PI()/4*F16^2*B$8/1000/0.75</f>
         <v>0.75388438018585902</v>
       </c>
       <c r="J16" s="220">
-        <f t="shared" ref="J16:J17" si="230">C16/B$8</f>
+        <f t="shared" ref="J16:J17" si="232">C16/B$8</f>
         <v>139.07738095238099</v>
       </c>
       <c r="K16" s="215">
-        <f t="shared" ref="K16:K17" si="231">(50+20)*2*PI()*B$12*C$16/LN(1+B$11*2/F16)/1000</f>
+        <f t="shared" ref="K16:K17" si="233">(50+20)*2*PI()*B$12*C$16/LN(1+B$11*2/F16)/1000</f>
         <v>1.6831237158895</v>
       </c>
       <c r="L16" s="214">
-        <f t="shared" ref="L16:L17" si="232">K16*24*180</f>
+        <f t="shared" ref="L16:L17" si="234">K16*24*180</f>
         <v>7271.0944526426601</v>
       </c>
       <c r="M16" s="218">
-        <f t="shared" ref="M16:M17" si="233">K16/E16*100</f>
+        <f t="shared" ref="M16:M17" si="235">K16/E16*100</f>
         <v>1.85893245792273</v>
       </c>
     </row>
@@ -66972,7 +66997,7 @@
         <v>500.67857142857201</v>
       </c>
       <c r="D17" s="214">
-        <f t="shared" si="225"/>
+        <f t="shared" si="227"/>
         <v>3.2261933049592901</v>
       </c>
       <c r="E17" s="215">
@@ -66980,35 +67005,35 @@
         <v>45.271244490784603</v>
       </c>
       <c r="F17" s="216">
-        <f t="shared" si="226"/>
+        <f t="shared" si="228"/>
         <v>0.015942071435193099</v>
       </c>
       <c r="G17" s="217">
-        <f t="shared" si="227"/>
+        <f t="shared" si="229"/>
         <v>0.023820074627992498</v>
       </c>
       <c r="H17" s="218">
-        <f t="shared" si="228"/>
+        <f t="shared" si="230"/>
         <v>11.9262009360652</v>
       </c>
       <c r="I17" s="219">
-        <f t="shared" si="229"/>
+        <f t="shared" si="231"/>
         <v>0.57133752214056399</v>
       </c>
       <c r="J17" s="220">
-        <f t="shared" si="230"/>
+        <f t="shared" si="232"/>
         <v>278.15476190476198</v>
       </c>
       <c r="K17" s="215">
-        <f t="shared" si="231"/>
+        <f t="shared" si="233"/>
         <v>1.4787421643890599</v>
       </c>
       <c r="L17" s="214">
-        <f t="shared" si="232"/>
+        <f t="shared" si="234"/>
         <v>6388.1661501607296</v>
       </c>
       <c r="M17" s="218">
-        <f t="shared" si="233"/>
+        <f t="shared" si="235"/>
         <v>3.2664049354553799</v>
       </c>
     </row>
@@ -67322,7 +67347,7 @@
         <v>250.33928571428601</v>
       </c>
       <c r="D23" s="214">
-        <f t="shared" si="225"/>
+        <f t="shared" si="227"/>
         <v>3.2261933049592901</v>
       </c>
       <c r="E23" s="215">
@@ -67330,35 +67355,35 @@
         <v>45.271244490784603</v>
       </c>
       <c r="F23" s="216">
-        <f t="shared" ref="F23:F24" si="234">(E16*4/PI()/4.2/(60-30)/1000/B$8)^0.5</f>
+        <f t="shared" ref="F23:F24" si="236">(E16*4/PI()/4.2/(60-30)/1000/B$8)^0.5</f>
         <v>0.0225454936359708</v>
       </c>
       <c r="G23" s="217">
-        <f t="shared" ref="G23:G24" si="235">0.216/((B$8/2)*F16/((1.5556*EXP(-0.0318393*B$9)+0.2374))/10^(-6))^0.2*1/(F16)*(B$8/2)^2*(-0.0040125*B$9^2-0.028625*B$9+1000.3875)/2/100000</f>
+        <f t="shared" ref="G23:G24" si="237">0.216/((B$8/2)*F16/((1.5556*EXP(-0.0318393*B$9)+0.2374))/10^(-6))^0.2*1/(F16)*(B$8/2)^2*(-0.0040125*B$9^2-0.028625*B$9+1000.3875)/2/100000</f>
         <v>0.0045130602161452798</v>
       </c>
       <c r="H23" s="218">
-        <f t="shared" ref="H23:H24" si="236">G23*C$16*2</f>
+        <f t="shared" ref="H23:H24" si="238">G23*C$16*2</f>
         <v>2.2595925417907399</v>
       </c>
       <c r="I23" s="219">
-        <f t="shared" ref="I23:I24" si="237">H23*10^5*PI()/4*F23^2*B$8/1000/0.75</f>
+        <f t="shared" ref="I23:I24" si="239">H23*10^5*PI()/4*F23^2*B$8/1000/0.75</f>
         <v>0.21649643684436401</v>
       </c>
       <c r="J23" s="220">
-        <f t="shared" ref="J23:J24" si="238">C23/B$8*2</f>
+        <f t="shared" ref="J23:J24" si="240">C23/B$8*2</f>
         <v>278.15476190476198</v>
       </c>
       <c r="K23" s="215">
-        <f t="shared" ref="K23:K24" si="239">(50+20)*2*PI()*B$12*C$16/LN(1+B$11*2/F23)/1000</f>
+        <f t="shared" ref="K23:K24" si="241">(50+20)*2*PI()*B$12*C$16/LN(1+B$11*2/F23)/1000</f>
         <v>1.6831237158895</v>
       </c>
       <c r="L23" s="214">
-        <f t="shared" ref="L23:L24" si="240">K23*24*180</f>
+        <f t="shared" ref="L23:L24" si="242">K23*24*180</f>
         <v>7271.0944526426601</v>
       </c>
       <c r="M23" s="218">
-        <f t="shared" ref="M23:M24" si="241">K23/E23*100</f>
+        <f t="shared" ref="M23:M24" si="243">K23/E23*100</f>
         <v>3.7178649158454702</v>
       </c>
     </row>
@@ -67371,7 +67396,7 @@
         <v>500.67857142857201</v>
       </c>
       <c r="D24" s="214">
-        <f t="shared" si="225"/>
+        <f t="shared" si="227"/>
         <v>3.2261933049592901</v>
       </c>
       <c r="E24" s="215">
@@ -67379,35 +67404,35 @@
         <v>22.635622245392302</v>
       </c>
       <c r="F24" s="216">
-        <f t="shared" si="234"/>
+        <f t="shared" si="236"/>
         <v>0.015942071435193099</v>
       </c>
       <c r="G24" s="217">
-        <f t="shared" si="235"/>
+        <f t="shared" si="237"/>
         <v>0.0068405201352704</v>
       </c>
       <c r="H24" s="218">
-        <f t="shared" si="236"/>
+        <f t="shared" si="238"/>
         <v>3.4249018491555598</v>
       </c>
       <c r="I24" s="219">
-        <f t="shared" si="237"/>
+        <f t="shared" si="239"/>
         <v>0.16407361795773701</v>
       </c>
       <c r="J24" s="220">
-        <f t="shared" si="238"/>
+        <f t="shared" si="240"/>
         <v>556.30952380952397</v>
       </c>
       <c r="K24" s="215">
-        <f t="shared" si="239"/>
+        <f t="shared" si="241"/>
         <v>1.4787421643890599</v>
       </c>
       <c r="L24" s="214">
-        <f t="shared" si="240"/>
+        <f t="shared" si="242"/>
         <v>6388.1661501607296</v>
       </c>
       <c r="M24" s="218">
-        <f t="shared" si="241"/>
+        <f t="shared" si="243"/>
         <v>6.5328098709107598</v>
       </c>
     </row>
@@ -67692,15 +67717,15 @@
         <v>1</v>
       </c>
       <c r="N2" s="142">
-        <f t="shared" ref="N2:N9" si="242">IF(M2=1,K2*50/35,K2*30/42)</f>
+        <f t="shared" ref="N2:N9" si="244">IF(M2=1,K2*50/35,K2*30/42)</f>
         <v>348.57142857142901</v>
       </c>
       <c r="O2" s="142">
-        <f t="shared" ref="O2:O9" si="243">IF(M2=1,L2*50/35,L2*30/42)</f>
+        <f t="shared" ref="O2:O9" si="245">IF(M2=1,L2*50/35,L2*30/42)</f>
         <v>870</v>
       </c>
       <c r="P2" s="142">
-        <f t="shared" ref="P2:P9" si="244">N2*O2</f>
+        <f t="shared" ref="P2:P9" si="246">N2*O2</f>
         <v>303257.14285714302</v>
       </c>
       <c r="Q2" s="142"/>
@@ -67782,15 +67807,15 @@
         <v>1</v>
       </c>
       <c r="N3" s="142">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v>1285.7142857142901</v>
       </c>
       <c r="O3" s="142">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>91.428571428571402</v>
       </c>
       <c r="P3" s="142">
-        <f t="shared" si="244"/>
+        <f t="shared" si="246"/>
         <v>117551.02040816301</v>
       </c>
       <c r="Q3" s="142"/>
@@ -67872,15 +67897,15 @@
         <v>1</v>
       </c>
       <c r="N4" s="142">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v>348.57142857142901</v>
       </c>
       <c r="O4" s="142">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>207.142857142857</v>
       </c>
       <c r="P4" s="142">
-        <f t="shared" si="244"/>
+        <f t="shared" si="246"/>
         <v>72204.081632653106</v>
       </c>
       <c r="Q4" s="142"/>
@@ -67964,15 +67989,15 @@
         <v>1</v>
       </c>
       <c r="N5" s="142">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v>900</v>
       </c>
       <c r="O5" s="142">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>388.57142857142901</v>
       </c>
       <c r="P5" s="142">
-        <f t="shared" si="244"/>
+        <f t="shared" si="246"/>
         <v>349714.28571428597</v>
       </c>
       <c r="Q5" s="142"/>
@@ -68056,15 +68081,15 @@
         <v>1</v>
       </c>
       <c r="N6" s="142">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v>157.142857142857</v>
       </c>
       <c r="O6" s="142">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>500</v>
       </c>
       <c r="P6" s="142">
-        <f t="shared" si="244"/>
+        <f t="shared" si="246"/>
         <v>78571.428571428594</v>
       </c>
       <c r="Q6" s="142">
@@ -68141,14 +68166,14 @@
         <v>452</v>
       </c>
       <c r="E7" s="239">
-        <f t="shared" ref="E7:E8" si="245">I7*I$35</f>
+        <f t="shared" ref="E7:E8" si="247">I7*I$35</f>
         <v>178.60133630289499</v>
       </c>
       <c r="F7" s="239">
         <v>179</v>
       </c>
       <c r="G7" s="239">
-        <f t="shared" ref="G7:G8" si="246">F7*0.9485</f>
+        <f t="shared" ref="G7:G8" si="248">F7*0.9485</f>
         <v>169.78149999999999</v>
       </c>
       <c r="H7" s="237">
@@ -68170,15 +68195,15 @@
         <v>1</v>
       </c>
       <c r="N7" s="239">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v>614.28571428571399</v>
       </c>
       <c r="O7" s="239">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>514.28571428571399</v>
       </c>
       <c r="P7" s="239">
-        <f t="shared" si="244"/>
+        <f t="shared" si="246"/>
         <v>315918.36734693899</v>
       </c>
       <c r="Q7" s="239">
@@ -68253,14 +68278,14 @@
         <v>1</v>
       </c>
       <c r="E8" s="142">
-        <f t="shared" si="245"/>
+        <f t="shared" si="247"/>
         <v>323.71492204899801</v>
       </c>
       <c r="F8" s="142">
         <v>324</v>
       </c>
       <c r="G8" s="142">
-        <f t="shared" si="246"/>
+        <f t="shared" si="248"/>
         <v>307.31400000000002</v>
       </c>
       <c r="H8" s="53">
@@ -68282,15 +68307,15 @@
         <v>2</v>
       </c>
       <c r="N8" s="142">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v>278.57142857142901</v>
       </c>
       <c r="O8" s="142">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>278.57142857142901</v>
       </c>
       <c r="P8" s="142">
-        <f t="shared" si="244"/>
+        <f t="shared" si="246"/>
         <v>77602.040816326495</v>
       </c>
       <c r="Q8" s="142" t="s">
@@ -68378,15 +68403,15 @@
         <v>2</v>
       </c>
       <c r="N9" s="142">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v>442.857142857143</v>
       </c>
       <c r="O9" s="142">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>385.71428571428601</v>
       </c>
       <c r="P9" s="142">
-        <f t="shared" si="244"/>
+        <f t="shared" si="246"/>
         <v>170816.32653061199</v>
       </c>
       <c r="Q9" s="142">
@@ -68490,15 +68515,15 @@
         <v>1</v>
       </c>
       <c r="N10" s="239">
-        <f t="shared" ref="N10:N31" si="247">IF(M10=1,K10*50/35,K10*30/42)</f>
+        <f t="shared" ref="N10:N31" si="249">IF(M10=1,K10*50/35,K10*30/42)</f>
         <v>285.71428571428601</v>
       </c>
       <c r="O10" s="239">
-        <f t="shared" ref="O10:O31" si="248">IF(M10=1,L10*50/35,L10*30/42)</f>
+        <f t="shared" ref="O10:O31" si="250">IF(M10=1,L10*50/35,L10*30/42)</f>
         <v>842.857142857143</v>
       </c>
       <c r="P10" s="239">
-        <f t="shared" ref="P10:P31" si="249">N10*O10</f>
+        <f t="shared" ref="P10:P31" si="251">N10*O10</f>
         <v>240816.32653061199</v>
       </c>
       <c r="Q10" s="239" t="s">
@@ -68585,15 +68610,15 @@
         <v>1</v>
       </c>
       <c r="N11" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>242.857142857143</v>
       </c>
       <c r="O11" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>1071.42857142857</v>
       </c>
       <c r="P11" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>260204.08163265299</v>
       </c>
       <c r="Q11" s="239">
@@ -68693,15 +68718,15 @@
         <v>2</v>
       </c>
       <c r="N12" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>396.42857142857099</v>
       </c>
       <c r="O12" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>432.857142857143</v>
       </c>
       <c r="P12" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>171596.93877551</v>
       </c>
       <c r="Q12" s="142" t="s">
@@ -68785,15 +68810,15 @@
         <v>2</v>
       </c>
       <c r="N13" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>335.71428571428601</v>
       </c>
       <c r="O13" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>142.857142857143</v>
       </c>
       <c r="P13" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>47959.183673469401</v>
       </c>
       <c r="Q13" s="142">
@@ -68895,15 +68920,15 @@
         <v>2</v>
       </c>
       <c r="N14" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>357.142857142857</v>
       </c>
       <c r="O14" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>150</v>
       </c>
       <c r="P14" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>53571.428571428602</v>
       </c>
       <c r="Q14" s="239" t="s">
@@ -68990,15 +69015,15 @@
         <v>2</v>
       </c>
       <c r="N15" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>235.71428571428601</v>
       </c>
       <c r="O15" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>300</v>
       </c>
       <c r="P15" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>70714.285714285696</v>
       </c>
       <c r="Q15" s="239" t="s">
@@ -69085,15 +69110,15 @@
         <v>2</v>
       </c>
       <c r="N16" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>121.428571428571</v>
       </c>
       <c r="O16" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>85.714285714285694</v>
       </c>
       <c r="P16" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>10408.163265306101</v>
       </c>
       <c r="Q16" s="239" t="s">
@@ -69182,15 +69207,15 @@
         <v>2</v>
       </c>
       <c r="N17" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>237.857142857143</v>
       </c>
       <c r="O17" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>313.57142857142901</v>
       </c>
       <c r="P17" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>74585.204081632706</v>
       </c>
       <c r="Q17" s="239" t="s">
@@ -69277,15 +69302,15 @@
         <v>2</v>
       </c>
       <c r="N18" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>357.142857142857</v>
       </c>
       <c r="O18" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>428.57142857142901</v>
       </c>
       <c r="P18" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>153061.224489796</v>
       </c>
       <c r="Q18" s="239" t="s">
@@ -69372,15 +69397,15 @@
         <v>2</v>
       </c>
       <c r="N19" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>307.142857142857</v>
       </c>
       <c r="O19" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>192.857142857143</v>
       </c>
       <c r="P19" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>59234.693877550999</v>
       </c>
       <c r="Q19" s="239">
@@ -69484,15 +69509,15 @@
         <v>2</v>
       </c>
       <c r="N20" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>714.28571428571399</v>
       </c>
       <c r="O20" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>250</v>
       </c>
       <c r="P20" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>178571.42857142899</v>
       </c>
       <c r="Q20" s="142" t="s">
@@ -69578,15 +69603,15 @@
         <v>2</v>
       </c>
       <c r="N21" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>571.42857142857099</v>
       </c>
       <c r="O21" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>371.42857142857099</v>
       </c>
       <c r="P21" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>212244.89795918399</v>
       </c>
       <c r="Q21" s="142">
@@ -69684,15 +69709,15 @@
         <v>2</v>
       </c>
       <c r="N22" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>396.42857142857099</v>
       </c>
       <c r="O22" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>396.42857142857099</v>
       </c>
       <c r="P22" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>157155.61224489799</v>
       </c>
       <c r="Q22" s="239" t="s">
@@ -69778,15 +69803,15 @@
         <v>2</v>
       </c>
       <c r="N23" s="239">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>500</v>
       </c>
       <c r="O23" s="239">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>157.142857142857</v>
       </c>
       <c r="P23" s="239">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>78571.428571428594</v>
       </c>
       <c r="Q23" s="239">
@@ -69887,15 +69912,15 @@
         <v>1</v>
       </c>
       <c r="N24" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>1428.57142857143</v>
       </c>
       <c r="O24" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>857.142857142857</v>
       </c>
       <c r="P24" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>1224489.7959183699</v>
       </c>
       <c r="Q24" s="142" t="s">
@@ -69988,15 +70013,15 @@
         <v>1</v>
       </c>
       <c r="N25" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>1357.1428571428601</v>
       </c>
       <c r="O25" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>828.57142857142901</v>
       </c>
       <c r="P25" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>1124489.7959183699</v>
       </c>
       <c r="Q25" s="142" t="s">
@@ -70085,15 +70110,15 @@
         <v>1</v>
       </c>
       <c r="N26" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>805.71428571428601</v>
       </c>
       <c r="O26" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>884.28571428571399</v>
       </c>
       <c r="P26" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>712481.63265306095</v>
       </c>
       <c r="Q26" s="142" t="s">
@@ -70182,15 +70207,15 @@
         <v>1</v>
       </c>
       <c r="N27" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>894.28571428571399</v>
       </c>
       <c r="O27" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>680</v>
       </c>
       <c r="P27" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>608114.28571428603</v>
       </c>
       <c r="Q27" s="142" t="s">
@@ -70277,15 +70302,15 @@
         <v>1</v>
       </c>
       <c r="N28" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>475.71428571428601</v>
       </c>
       <c r="O28" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>814.28571428571399</v>
       </c>
       <c r="P28" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>387367.34693877603</v>
       </c>
       <c r="Q28" s="142" t="s">
@@ -70372,15 +70397,15 @@
         <v>1</v>
       </c>
       <c r="N29" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>445.71428571428601</v>
       </c>
       <c r="O29" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>775.71428571428601</v>
       </c>
       <c r="P29" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>345746.93877551</v>
       </c>
       <c r="Q29" s="142" t="s">
@@ -70465,15 +70490,15 @@
         <v>1</v>
       </c>
       <c r="N30" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>428.57142857142901</v>
       </c>
       <c r="O30" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>857.142857142857</v>
       </c>
       <c r="P30" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>367346.93877551</v>
       </c>
       <c r="Q30" s="142" t="s">
@@ -70558,15 +70583,15 @@
         <v>1</v>
       </c>
       <c r="N31" s="142">
-        <f t="shared" si="247"/>
+        <f t="shared" si="249"/>
         <v>158.57142857142901</v>
       </c>
       <c r="O31" s="142">
-        <f t="shared" si="248"/>
+        <f t="shared" si="250"/>
         <v>542.857142857143</v>
       </c>
       <c r="P31" s="142">
-        <f t="shared" si="249"/>
+        <f t="shared" si="251"/>
         <v>86081.632653061301</v>
       </c>
       <c r="Q31" s="142">

</xml_diff>